<commit_message>
Get daily reddit data: Mon Nov 13 08:06:32 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,23 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>17u5yix</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Classic french ombre 💅</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17u5yix</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get weekly top reddit data: Mon Nov 13 08:09:29 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="top" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5570,4 +5571,4647 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C272"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>image_url</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>17sqctf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rate my nail tech 💅🏻</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sqctf</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>17rbjc8</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5 month progress doing my own nails :)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rbjc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>17s540s</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Some nails my girlfriend did that I’m really proud of</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17s540s</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>17svvqy</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Started doing my own nails recently, what do you guys think? :)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8g0ilaeeqzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>17q90rk</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Disappointed</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q90rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>17qx1ns</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>My nail tech kills it every time</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qx1ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>17qrs64</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ethereal skies 🌙☁️</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byilpapu06zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>17pr1sw</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Got my nails did! wanted something bright and girly this time 🍓💗</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pr1sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>17pjqx8</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>My nails in 2021 (top) vs. today (bottom)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc6tgvmk3uyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17oy10q</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Witchy snake skin nails by me 🐍</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17oy10q</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>17pcjts</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>My boyfriend just referred to this as a “nail garage”</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lybbvwrmhsyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>17py0js</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Did my first refill ever on myself with gel, how did I do? 🌸</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktgtjz2zbyyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>17ty00s</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Nail tech said I’m in my hoe nails era 💅🏼✨</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2q9snu71d00c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>17si4z1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>I started doing my own nails during the pandemic. Sharing a few of my favourites!</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17si4z1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>17sb5kt</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>My nail lady slayed per usual for these Christmas nails🤭(yes Ik it’s early,these are for family Christmas pics)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sb5kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>17s6qbf</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>I think these might be my favourite nails I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6x1z5nojjzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17tawz6</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sparkly cloud nails ☁️ ✨</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvjj7b4uztzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>17qor0k</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>My nails matched my hoodie today 💗</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fui9byzhc5zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>17qokmt</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>"Cruella de Vil" Ombre by me</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1zirqmhya5zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>17s20nz</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Found nails I did about 8 years ago. Excuse the image quality from an old phone</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17s20nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>17tjjh7</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Been doing my own nails for a while and I’m proud of my recent work!</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tjjh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>17tadga</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>My Wedding Nails! It’s only a few days away😭🤍</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tadga</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>17t3ezh</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>My nail lady is amazing</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p1a2cc96szb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>17qjtg0</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Got my nails done for the third time ever :)!</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akyxd1cq24zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>17psk9w</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Is there a way to use this type of polish without globing it on?</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17psk9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>17tqwdp</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Just did my nails to celebrate getting a new fully remote job with much higher pay than my last remote job! 💖</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a4u6ieyryzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>17sxsec</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Rate my nail tech please 😊</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sxsec</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>17rmdzj</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Tis the season for glitters!</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/042bgxgzudzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>17qtwpf</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>My 4 year old said I should choose “dark jade” today 🤩</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ji3xf6mmh6zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>17sgozv</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Got my nails done in Ktown</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxyjfxaaslzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>17qxhn7</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Gemstone nails 💎✨ did an ombre french first and felt so plain I had to liven it up</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qxhn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>17swr8r</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>My best friend is a nail tech</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8vf4cpzlqzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>17tpjtt</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>pink &amp; blue set on my little sister :)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tpjtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>17ri2wz</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Too early for Christmas nails?</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ri2wz</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>17riwkk</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>I have so many colours and designs I want to try, but I always fall back to neutrals 🫶</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17riwkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>17p9p2q</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>I love my new stamping plate</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/73y6ep7mvryb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17sfuzs</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>I decided to do my nails like Carmela on the Sopranos and i really like them</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6onwdidllzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>17r3654</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>I love my nail tech so much</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64veqidqk8zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>17qdnyx</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Y’all like my Foxxy Fall nails?</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qdnyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>17tqnhg</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Am I crazy, or are my nails crooked?</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tqnhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>17rjpqm</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>I am learning how to do my own nails, I just wanted to show some sets I’ve done.</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rjpqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17r1r3f</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>What the heck am I doing wrong? 😒</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdf6m0jb88zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>17soqgm</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>taking a small break from my go to pinks for a pop of purple 💜</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bhyx376jynzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>17q6hl4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Bit late for Halloween nails but I just wanted to show where I was a couple of years ago to now. Not everyone is blessed with talent, some of us have to work hard but it pays off eventually! My skills are improving all of the time and I’m so proud of where I am now. Don’t ever give up!</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nhwh9lja50zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>17tcch2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Collection of all my recent nails (all my natural nail with regular gel polish)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tcch2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>17poe4x</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Shego nails💚🖤</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17poe4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17t3tr3</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>It's my bday today! Made myself some scorpio season nails 🦂</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aojbcjm9szb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17qayze</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>What nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qayze</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>17s7x8w</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>i call these my blue’s clues nails :)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd2cqia8tjzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>17p5dwy</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>I’m in love with this color that I’ve never worn before, what should I wear next time?💚</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17p5dwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>17rniux</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Natural nails have been strengthened and lengthened!</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulhnfgy24ezb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>17skkxo</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>I’m usually a pink kinda girly…</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ejji208qmzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>17raauy</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Choc glaze BIAB 🍩</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17raauy</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>17pzkur</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Would another nail shape suit me better?</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pzkur</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>17q5z88</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>🦋Butterfly Nails &amp; mourning my dead pointer nail🦋</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q5z88</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>17syw5m</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Yesterday's mani ;) let me know what you think</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17syw5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>17tvmmb</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Lastest sets from last week 🫶🏼💅🏼</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tvmmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>17sdcs4</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sdcs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>17rmlr6</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Super proud of how well I painted with my non-dominant hand this time!</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejh3c4arwdzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>17sj0wr</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Studio Ghibli Howl's Moving Castle nail set 🌟</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sj0wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>17tx9fu</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Does anyone know what polish this is?</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tx9fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>17rfjyr</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Kiss Salon Acrylic Leilani</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rfjyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>17qlf3z</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>did my own gel nails and extensions for the first time with kokoist products!</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qlf3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>17qqg7m</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Midnight blue 💙🖤</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1k3orkd8q5zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>17t7qbx</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>💕 Cinnamoroll nails 💕 That line work!!</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wokyxttl5tzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>17pireb</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Not perfect but done by my sister 😊</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pireb</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>17sf16v</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>What do you think of these nails?</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sf16v</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>17rr9wr</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1 coat funny bunny 2 coats bubble bath is elite!💅🏼🫧✨</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/569t25l8yezb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>17qjjmm</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>birthday nails</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qjjmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>17p6a2k</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Floral Gel Nails by my Mom ♡</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo1eirec5ryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>17qo5px</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vls9mbpr75zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>17rrz8x</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>"Low-key Pumpkins with a Dash of Petals" by me</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9c4x8v34fzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>17s61vc</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Glazed Frenchies</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17s61vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>17p5z1x</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Is this a good nail shape for me?</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7dlmb5y2ryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>17rh1vq</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>What's the point of 10 nails if not 10 different designs?</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rh1vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>17t6eb8</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Which pic is best? 1 or 2?</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t6eb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>17q9ze9</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>When made my nails match my hair</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18689g95y0zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>17pr8md</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>New nails! My lines aren’t that clean yet and it takes me ages but I love them</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pr8md</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>17po3xl</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Fresh set done at chichi nails in Ontario Canada - by far my most favourite 🌊 🐟 🥶 ❄️</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tzifz32dvyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>17sjl5i</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>My nail tech is awesome!!</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkf9y6o9hmzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>17r2bze</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>getting bored of nails after 3 days</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17r2bze/getting_bored_of_nails_after_3_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>17qfsz7</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>11 month consistent work and improvement!what do we think?</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qfsz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>17syl74</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>First time getting gel - is it time to remove it? Not sure how much grow out is acceptable before it looks bad.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17syl74</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>17q194l</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Color of the week</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tbmejqb1zyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>17qzwu7</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>November = Snowflakes</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4sa78fas7zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>17tiyy8</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Depression tried to stop me yesterday. I said no. And used it to Channel even more creativity. 💕 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8i7gyx6brwzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>17qptkr</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>🍫</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzj5mio1l5zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>17sxcf0</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Dark fairy vibes</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sxcf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>17swhif</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>"Da ba dee da ba di" by me!</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17swhif</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>17p1q4m</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>I’m self taught. Still learning how to get an apex right. Any tips and tricks?</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17p1q4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>17t831o</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Kawaii Nails!</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7noy13s8tzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>17p6zbk</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Do you like long sharp nails? I do !</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9mmqa6yaryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>17ph7qm</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Forgot to post the finished product</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ph7qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>17ttyvv</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Did the nail tech do a good job?</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ttyvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>17u2bx6</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Dark emerald green that I got done today</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17u2bx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>17t3sgc</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>❄️✨</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t3sgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>17s95mx</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>the most “natural” you’ll ever see my nails. builder gel mani on me by me!</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzmbhe013kzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>17t9e3n</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Moody Fall/Winter goodness</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t9e3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>17sumpf</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>I’m a beginner, just started studying nails, tips?</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqaqkckv2qzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>17sldr4</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>How would you politely tell a nail tech that you prefer a quiet service?</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17sldr4/how_would_you_politely_tell_a_nail_tech_that_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>17p8lce</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>We all know this kind of pain..</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5byeqvv9nryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>17qs909</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>The finest holographic polish…</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qs909</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>17s94dr</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>I saw Cady Heron wearing House of Hades and flip-flops, so I bought House of Hades and flip-flops</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ense5pr2kzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>17rjrh3</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>💛🤧Ricola🤧💛</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rjrh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>17tx9fc</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>While on the hunt for a perfect milky white, I stumbled upon a nice, neutral ynbb</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tx9fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>17qrwah</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>House of Hades</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihv6inbs16zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>17q32tp</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Playing cards ♡♧◇♤</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q32tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>17syaqi</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Thoughts on Holo Taco After Party collection? (Swatches by the company)</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcorinmdzqzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>17psfn3</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Bella where the hell have you been loca?!</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17psfn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>17pbzvg</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>So cozy ☕💜</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pbzvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>17sgz4c</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>If there’s one thing I’m absolutely feral about it’s a subtle polish with a blue shimmer</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sgz4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>17q0ern</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>The perfect bougainvillea shade!</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c08h8zctuyyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>17sawho</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>"Which color will you wear next?" "Yes."</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sawho</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>17pu5lv</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Any suggestions on non-gel polishes that could give the jelly/ombré effect? Or would mixing up regular polish with clear be best to get that smooth transparency transition?</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1r6zc2mfxyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>17p3dgd</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Rainbow gradient crackle</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj0ovdophqyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>17saiwn</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Had to hop on the sassy sauce train because no amount of purple shifties are enough</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17saiwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>17rdtak</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>My only adjective is “Angelic”</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rdtak</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>17qwpei</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>My husband said my nails look like beetles and I have to agree</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9zqttv837zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>17p497o</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>My Mooncat sale order is already here!</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz43h821pqyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>17tutd2</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Urban Decay Gash (1996)</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpjbg7a6nzzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>17oy74g</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Witchy snake nails by me 🐍✨</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17oy74g</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>17reidu</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Well... this IS a dumb question....is this the same polish????</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17reidu</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>17tcumc</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>I bought 'em all, might as well wear 'em all</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tcumc</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>17r1ai8</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>My first Mooncat order... Is this normal?</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17r1ai8</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>17to8nn</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Korean Tiger</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17to8nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>17s6j7l</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Me watching everyone else get their Mooncat orders really fast</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n58l3p83ijzb1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>17rukl2</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>When you can’t decide on a color…</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rukl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>17q9rgw</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>How do people feel about Holo Taco?</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17q9rgw/how_do_people_feel_about_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>17pvrtl</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>SEAWEED FINGIES!! 💚😻</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4w6mjirtxyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>17szm3u</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Anyone else excited about Lūmen’s release on Monday?</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17szm3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>17t8a7t</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Changed my nail shape after like 5 years 🙈</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t8a7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>17tkmrl</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Colored pencil shavings ✏️</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppcarpud9xzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>17qreef</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>"Cruella de Vil" Ombre by me</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9232vujqx5zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>17t9ujb</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>ILNP Spiced Cider + Bear Hug 🤎</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t9ujb</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>17qnf5j</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Nail Polish Swatch File Part 2: Full Flip through</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hmaz8e7i15zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>17q3i7s</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Would anyone be interested in a twice a week (probably every Monday and Friday) check-in post for those no a low buy or no buy during the holiday season?</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17q3i7s/would_anyone_be_interested_in_a_twice_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>17s8vve</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Trying to channel the vibe my neighborhood is setting</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17s8vve</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>17swet2</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>I've never used Zoya, but this looks like a great deal!</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fonwlwyiqzb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>17t46y0</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Pink fairy lights</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvahp5ykcszb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>17s56k8</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Ethereal’s Vanitas ✨</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fi008zkf6jzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>17sd1rm</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Operation: Shop your stash - Weekly Challenge 💅</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17sd1rm/operation_shop_your_stash_weekly_challenge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>17pfknu</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Nail Photo Bomber</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wak28rjz3tyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>17suoby</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>New favorite magnet combo feat: ILNP Shooting Star</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17suoby</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>17s5wt2</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Absolutely IN LOVE</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17s5wt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>17tpo6d</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>🍄Widdle Mushies🍄</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tpo6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>17q1zm3</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>one polish, lots of colors!!</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q1zm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>17p7ovu</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>chocolate nails! 🍫</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40kri1scgryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>17t4kj4</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>New favorite red unlocked</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf0v2khgfszb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>17qlqbk</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>What's the consensus on ILNP Real Magic shimmers and flakies?</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6dz6n7fm4zb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>17phbsz</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Fancy Gloss - Ironic - why is this thermal so good??</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wnft867cityb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>17s5ac5</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Is anyone else so bored with BKL lately? I feel bad saying it but what gives?</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcv9mued7jzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>17pmgvp</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>I understand the holo hype completely now.</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxfucjtvtuyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>17p9iup</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Nail Polish Swatch File</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17p9iup</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>17quq2t</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>🐉A dragon without its rider is a tragedy. A rider without their dragon is dead. 🌩</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zotojwn6o6zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>17q5r8x</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>anyone else have a go-to first date nail strategy? i usually go for something subtle but fun</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lmpt1bvzzyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>17rmtzj</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>ILNP Spiced Cider</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rmtzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>17qusmx</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>House of Hades 💙</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qusmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>17tlsvw</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>🌸</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tlsvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>17ro7b7</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Thought the china glaze was a dupe as I walked past, but turned out quite different</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1e2nsg9d9ezb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>17tnl6k</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Anyone else’s Zoya order get cancelled?!</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytao98kyzxzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>17qkhv7</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Perfect color for a lunch out! I On Nails, Expressie Streetwear n' Tear, #339, and finished with Seche Vite.</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qkhv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>17t4fbk</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Deep Space by ILNP</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/st050g49eszb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>17q9bbu</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Birefringence 💙💜</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q9bbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>17pj9u8</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Grandma's mani</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pj9u8</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>17si03l</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>H&amp;M Nail Polish is Actually REALLY Good 😳</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k05enjf3mzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>17txlag</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Tortie Skittle 🐢💕💜💙💚</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gm12ici900c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>17pe1kc</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Just a lil’ Haul</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h3zxrhjssyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>17p6lt4</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Sweater Nails for Sweater Weather</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnf9ieiy7ryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>17tlu2f</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>ILNP Comet… and trying a new to me nail shape?</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tlu2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>17riss1</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Rose Were The Days</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17riss1</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>17s7f8k</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>[Angry honking intensifies] 🪿🪿🪿</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czyphtw7pjzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>17pa6k5</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>I was a bit mean to linear holos</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fthv5sa6zryb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>17t6cwb</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Reflective blurple for my birthday</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t6cwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>17p4i2j</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>How do you choose what polish to wear?</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17p4i2j/how_do_you_choose_what_polish_to_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>17qwj8u</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Autumnal af</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qwj8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>17sd96u</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Fall green</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwfdwrsn0lzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>17p41j9</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Written Invitation 💜🍂🍁💜</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17p41j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>17rgjdh</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>So shifty 😍</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/286agsekkczb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>17rhece</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>So delicious I want to eat it</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn5rddadrczb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>17pg5zf</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Bag</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6ab477n8tyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>17qzlm4</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Y'all were right about ILNP Fairy Dust (shown in various lighting)</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nq2i7l8rp7zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>17smqoy</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>ILNP Cookie Cutter 🍪</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc0vbiyebnzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>17tvq5n</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Did mine and my mom's nails today!</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tvq5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>17to5eq</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Replicating gel designs with regular polish 💚🤎</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17to5eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>17qr4hr</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Decided to skip top coat..</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmfly3ehv5zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>17td7p6</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Marsala jelly nails</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b15xgq60puzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>17r31gh</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Mooncat - Dragon Scales 🐉</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17r31gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>17tet0l</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>ILNP Strawberry Shake</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tet0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>17pkip6</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>I'm a thermal convert 🔥 ❄️</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/weodrjziauyb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>17t4so3</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>LynBDesigns - Leaf it to me</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/acm2y5uahszb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>17sae08</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Cirque Colors making amends for Lucky Bag</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i1lghtzckzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>17r4muw</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>More Written Invitation Love</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jbqkmgpey8zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>17pjbvw</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>First attempt at reverse stamping!</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pjbvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>17pxlmr</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Who’s getting….</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqd2uq7m8yyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>17qpny4</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>My favorite froggehs</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmo5292uj5zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>17pvoeo</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>{PR} Love this combo!</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pvoeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>17pjxzy</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Kiss Me or Elf!</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whik1fgc5uyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>17t03cj</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>One of my fav polishes</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t03cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>17t397y</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>TMTYL and Fairy Dust comparison</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g2jopn9w4szb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>17pzm66</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Current claws</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dvtkcs3moyyb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>17r5zm0</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>I need a heaping spoonful of truth soup. Yay or nay to these press ons I made for a Disney cruise?</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17r5zm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>17oy2vg</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Witchy snake nails by me 🐍✨</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17oy2vg</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>17q7k3v</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>What style of art is this?</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q7k3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>17sbksb</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>First attempt at plaid</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2di52ekomkzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>17svpwg</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>My practice Auroranail attempts</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17svpwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>17q4ifn</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>A selection of my nails from this year.</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q4ifn</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>17pmwdq</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Winter makes me a bit 🍋 sour (in a good way) by me (@beowoofstudio)</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8cini3hyuyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>17rnlbs</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>“We might say that the earth has the spirit of growth; that its flesh is the soil.” — Leonardo da Vinci</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rnlbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>17t79ql</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>❄️✨</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t79ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>17pdz9k</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Fairies count for fall right? 😅</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhoasga2ssyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>17qzq35</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Winter polar bear</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xhbb7qrq7zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>17qp845</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>First time trying rainbow nails💿🌈</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qp845</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>17tmb9t</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Holiday set!! Done by Lynn @ M.Vince nails. Ft. Wayne IN.</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bhkq3droxzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>17qfawy</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know I’m late but my Halloween nails </t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nvqcy70ee2zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>17qhfcg</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>"Cruella de Vil" Ombre by me (ig: beowoofstudio)</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qhfcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>17rm52o</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>First official set I painted on my mom, what do you think</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkovi0zxsdzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>17rcja1</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Some fall baddies!</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rcja1</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>17sj1w5</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Howl's Moving Castle nail set 🌟💙🌟</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17sj1w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>17q8ixn</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>we can’t skip over Thanksgiving!</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qu9vvmpl0zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>17pv3x7</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Freehand Mushroom Nail Art</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2qgbln3oxyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>17pynsf</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Black bear set</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pynsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>17p6yab</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>✨️ First set of press on nails!</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17p6yab</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>17sc4u3</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Done by J at Dluxe nails in Chicago</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t668juh9rkzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>17qw9hm</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Simple nail set</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ccz7o5yz6zb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>17swil8</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Fall Nails</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17swil8</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>17tnkjb</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Artsy Skittle</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fi9iw0yszxzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>17rm2fq</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>My nail tech is my soulmate</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rm2fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>17rmk7w</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Anyone else love pandas?</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17rmk7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>17rj0v4</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Nails to honor the passing of a birder. 🐦‍⬛🖤</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj4uuqs24dzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>17tb2xt</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Swarovski Crystal stilettos</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0qiic4ni1uzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>17sq3vz</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Got my toenails done, how do you like the design ? Done by Ruby Nail Salon, Shanghai</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zl6ohgndhozb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>17qeu3r</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Recently graduated nail tech! I've been doing a lot of practice art in between clients 💖</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qeu3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>17tw1se</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Went for one thing cute this time!!!</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tw1se</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>17tj5tr</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>"Put on your red shoes and dance the blues" by me (ig: beowoofstudio)</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nswdluintwzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>17p33lv</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Missed having some bling on my nails</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xsv04iafqyb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>17t12du</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Experiment with jelly nails</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17t12du</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>17s215x</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>First attempt at “designs”</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9gd322gaizb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>17sk461</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainbow ones with glitter </t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1j2y0hjylmzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>17sd7hm</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Fall greens</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9qm1xc80lzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>17pxc7f</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Chrome Comic</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17pxc7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>17saery</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Rainbows by TS Nail Spa, Panama City Beach!</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lthhd9l6dkzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>17plhss</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Let it snow</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ns88q5njuyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>17twk2g</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>blue nail design 🦋 done at chichi nails in Canada Ontario 🧼 💅</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x16n2cw000c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>17sb7ip</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Spooky Halloween press on set I made 🕸️👻</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydt79mzpjkzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>17qaq6e</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Edgar Allan Poe</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qaq6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>17pilhc</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>It’s gir! 💚 invader zim nails hand painted - chichi nails in Ontario Canada</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04ewia89ttyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>17szrlf</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting a Powerpuff girls character press on </t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d0s7ymazbrzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>17qdyav</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Water slip decals of my own paintings</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qdyav</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>17tyogn</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Most recent after not doing my nails in a while</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40j29811j00c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>17qq46g</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Any hockey fans around? My team needs good juju, this is my contribution 😂</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qq46g</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>17q9dke</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>"Who You Gonna Call?" by me (ig: @beowoofstudio)</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbg4qonus0zb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>17qgjo9</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>More of my nails</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qgjo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>17qbvz5</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Fall/ holiday nails</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qbvz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>17qf935</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Some of my latest nail art</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0438qxvtd2zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>17twlqm</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Maggie baby 👶🏼🤰🏻🤱🏻🍼 The Simpsons Character • hand drawn art done at ChiChi nails in Canada Ontario ✨</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5jw08y8100c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>17qmqbe</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Scroll right to see them glow</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17qmqbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>17tuo98</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17tuo98</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>17tne4x</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>First time for cat’s eye</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pldqfca9yxzb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>17q2ei5</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>💐 trying something new</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3ys5yacazyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>17snynf</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>"Friends" nails</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bh6vsti1pnzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>17q0ovk</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Can someone tell me how to do this style?</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8tnv7y0xyyb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>17pyq34</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>looking good? What I can do with this?</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8wxq0shhyyb1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>17q6h76</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Stained glass nails</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q6h76</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>17sh2qo</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Obsessed with this pattern</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmqd2wghvlzb1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>17qgwc7</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>hi I’m a complete newbie, and I’m looking to do this (@peaknail) on myself. Need a step by step procedure 🥹</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nxg27t9pz2zb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>17q5j0u</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Aurora Nails</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17q5j0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>17u488w</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Looking to recreate this set but i’m unsure if it has chrome powder on top to give it that finish. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9cc12qv120c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>17ssoni</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Magnetic Nail Polish</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17ssoni/magnetic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>17psl0t</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Many Reasons for a Festive Season</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17psl0t/many_reasons_for_a_festive_season/</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>17rdqg2</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Favourite YouTube tutorial sites?</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17rdqg2/favourite_youtube_tutorial_sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>17szhfs</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Green and Copper Fall Nails / Emerald Nails / Quick and Easy</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>https://youtu.be/RqWraDMMljo?si=rMHyxYcQde0rQLP-</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Get daily reddit data: Mon Nov 13 08:16:31 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C302"/>
+  <dimension ref="A1:C305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5565,6 +5565,57 @@
       <c r="C302" t="inlineStr">
         <is>
           <t>https://www.reddit.com/gallery/17u5yix</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>17u62u5</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>What to do when an acrylic nail breaks?😭</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17u62u5/what_to_do_when_an_acrylic_nail_breaks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>17u5zd8</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Did These Myself Tonight</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcle1p41p20c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>17u5zrp</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Orly Shining Armor Top Coat Issues?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17u5zrp/orly_shining_armor_top_coat_issues/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Get daily reddit data: Mon Nov 13 08:34:51 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C305"/>
+  <dimension ref="A1:C306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5616,6 +5616,23 @@
       <c r="C305" t="inlineStr">
         <is>
           <t>https://www.reddit.com/r/RedditLaqueristas/comments/17u5zrp/orly_shining_armor_top_coat_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>17u6561</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Staring a new job soon, are these nails nice/tame enough? I'm a UI designer and the company is "casual-ish"</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whd69h89r20c1.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Get daily reddit data: Tue Nov 14 08:08:24 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C306"/>
+  <dimension ref="A1:C467"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5633,6 +5633,2743 @@
       <c r="C306" t="inlineStr">
         <is>
           <t>https://i.redd.it/whd69h89r20c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>17ux90y</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>My first attempt at french manicure!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru99c07ep90c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>17uwe59</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Just got my nails done.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8i0buzde90c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>17uwb6y</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Professional quality?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uwb6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>17uveiz</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>It’s giving vampire queen 😍</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyygyrnz290c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>17uvbpm</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Ft. Milk</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uvbpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>17uursi</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Yay or nay? 🫶 ps. I did them myself!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqmxziiaw80c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>17utxg8</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Looking for dust collector recommendations</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17utxg8/looking_for_dust_collector_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>17utubv</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Self taught progress</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17utubv</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>17utghv</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>what are the best press-on nails for flat/weak nail beds?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17utghv/what_are_the_best_presson_nails_for_flatweak_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>17utflh</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Dark cherry nails 💅</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17utflh</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>17ut2yq</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Recent nail art I’ve done 😊</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ut2yq</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>17ut12s</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Nails by me</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks8sqh6se80c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>17ut0hk</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Nails by me</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qghrjwfne80c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>17urnck</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Scooby Doo Mystery Machine Inspired</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9ip30ie280c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>17upxik</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>OBSESSED .</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17upxik</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>17ukx32</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Wonky nails? What works be best?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otkpu7i1k60c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>17usnxz</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Did my nails for the holiday</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1qlxtshb80c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>17usl4t</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Coffin or almond</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17usl4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>17use93</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Glazed donuts nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g38zidt3980c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>17urtlw</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>My first time trying almond shape nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17urtlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>17urg3h</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Not too Christmasy right?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17urg3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>17urfpb</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Gel-X Designs</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17urfpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>17ur6x5</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjdmc0ehy70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>17ur1a6</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Anyone else obsessed with magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ur1a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>17uqysj</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Gameday Nails: Would you rock this design?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slys5t88w70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>17uqgi7</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>It sounds weird but does anyone have a 'favourite' nail??</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17uqgi7/it_sounds_weird_but_does_anyone_have_a_favourite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>17uq4ju</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Evil eye</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb6tipo2p70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>17upldg</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Did I make a good combination?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4xsntsek70c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>17upkv9</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>I need advice with broken nail</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p00g2r7bk70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>17updxy</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Sets that I made yesterday, 8 hours well spent</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17updxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>17upb94</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Learning to do my nails!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv2we92yh70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>17up44o</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Is Onyx Hard as Hoof a good buy for someone who doesn't have thin peeling nails?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17up44o/is_onyx_hard_as_hoof_a_good_buy_for_someone_who/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>17uorye</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Short, simple, and sweet (ft. bob)</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uorye</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>17uonid</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>My first time trying nail forms!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uonid</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>17uokwm</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Fresh set 🖤💛🤎</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8nr88avb70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>17uogus</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Ill call em dreamy princess nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uogus</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>17unxf0</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Yellowing nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17unxf0/yellowing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>17unexz</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>It’s giving chocolate caramel</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dq01bxfo270c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>17un0vu</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Fall colors</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnxtaavkz60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>17umokg</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>I want to get my nails done 🥺</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17umokg/i_want_to_get_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>17umlkz</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Started doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17umlkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>17um8z8</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17um8z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>17ul4p3</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>My first DIY BIAB fill.. did I do alright? I'm still not great at shaping almonds, but I think the apex looks alright!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ul4p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>17ukoni</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Birthday nails💅🏼</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sl0vbq3di60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>17ukomf</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>From a wedding I was recently in. Copied from a previous post (sorry forgot who it was!)</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53rqa5mdi60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>17ukd6f</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>I tried 😩</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qfff55ovf60c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>17uk25f</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Back to the basics - I love pink 🤭</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyhw9s0nd60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>17ujab9</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>No more acrylics!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vesajihm760c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>17uin8q</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Help? Advice</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qj0x0at260c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>17uil8j</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Just wasted $60 🥰🤪</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uil8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>17ugvd0</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Nails for the festive season</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhzrq8fdp50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>17uidqd</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Loving my new nail design!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/427hqjzw060c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>17uicd5</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>🌚Too much? 😅</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97n5psrm060c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>17uiagw</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>My newest set</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys69mxy8060c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>17ui1ld</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>"Take the Espresso" Expressie Quick Dry Polish</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ui1ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>17uhr90</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I just LOVE IT 💅❤️</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwpuaoc7w50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>17ug0gg</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I want them to be stronger, any advice? Should I get gel over them or something? Really don’t want them to break again.</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ug0gg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>17ufa3y</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Press on nails tips</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ufa3y/press_on_nails_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>17ue3ac</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Seeking tips to make my nail polish last</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ue3ac/seeking_tips_to_make_my_nail_polish_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>17ubd9q</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Top Coat doesn‘t get shiny? 😫 any ideas why!?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhv2jyszg40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>17ufvm8</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>went with the almond!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ufvm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>17ufrlv</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>When I do my nails with my dominant hand vs the non dominant hand 🥴</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ufrlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>17u6spa</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>What do people think about Gel wraps?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17u6spa</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>17ufn4o</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Love me some red ✨</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yady7bazf50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>17ufham</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Best glue for gelx? Some lasted 2 weeks, others started pulling up after a few days?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ufham/best_glue_for_gelx_some_lasted_2_weeks_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>17ufepm</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Got these press ons from OPI and I’m OBSESSED</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13fb7w25e50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>17ueqwv</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xvpc7ex850c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>17uepb4</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Cozy quilty nails</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uepb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>17uegqy</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Polka dots!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uegqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>17uda6z</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>A break from gel and dip nails</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uda6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>17ud2n9</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>I'm Dsypraxic and after lots of practice and a whole nail course I've finally been able to paint my nails without it looking a mess</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ud2n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>17ud1ce</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>space rock pimples - gel overlay on my natural nails</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ud1ce</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>17ucv5p</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>love my airbrushed cuties!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ucv5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>17ucf7t</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Lowkey Sharp claws</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g3zm3c8q40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>17ucd3c</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>it’s getting chilly bundle up. 🥶❄️✨</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7be2e3ipp40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>17uc2lw</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>My friend did a freestyle gel manicure on me, thoughts?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uc2lw</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>17uc1lq</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Square or round?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uc1lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>17ubky2</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Sistaco without lamp</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ubky2/sistaco_without_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>17ub6ak</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Regular gel polish dupe for ASP “Birthday Suit”</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ub6ak/regular_gel_polish_dupe_for_asp_birthday_suit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>17ub277</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>French tips I done myself :)</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zpuexn9e40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>17uaoac</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Very happy with my set!!</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uaoac</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>17u9dsm</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>How can I make my natural nails last longer?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0emcreejx30c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>17u8m8n</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>🕸</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz0jf0ilo30c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>17u8loo</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Something new</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99f0ijhdo30c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>17u7whc</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Not so bad for a first time I think</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ums9wzif30c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>17u7apo</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>press ons I made</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17u7apo</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>17u6oxz</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Very simple but I love it</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17u6oxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>17u6ihs</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>First set of red nails ever</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thm8ywsdw20c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>17ux2ex</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Does anyone else get really red swollen feet from standing all day?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ux2ex/does_anyone_else_get_really_red_swollen_feet_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>17uwsz4</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>leopard print nails</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5y74h5jj90c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>17uwr4b</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Too Much…Say Whaat?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hs5toivi90c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>17uvb77</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>RV There Yet?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uvb77</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>17uupnq</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>I really love Fall</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uupnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>17utv3k</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>In a Purple Mood 💜✨</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17utv3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>17uto59</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Cirque Colors Venetian Sky 💜💕✨</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uto59</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>17ut3tv</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Can you guess my favorite color😆</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ut3tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>17ut2yb</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>What I received in my Cirque lucky bag</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwoq0gx8f80c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>17usz9g</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Finally trying cherry mocha 🍒 ☕️</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17usz9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>17uriho</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Cirque Colors Indigo Jelly</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17uriho/cirque_colors_indigo_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>17us5no</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Sparkly french tips on a Gel X manicure</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebtk235q680c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>17urqjq</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Obsessed with Moonjelly</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5n8ifr6380c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>17urfj7</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Under water sparkle vibes</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzxujxak080c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>17ure10</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Your favorite nudes that have ✨razzle dazzle✨</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ure10/your_favorite_nudes_that_have_razzle_dazzle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>17ur5yf</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>ILNP NYE Collection from last year! Skittle style :)</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ur5yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>17ur2dp</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>How Do You Organize?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4t9qd9cx70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>17uqt8v</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Mooncat ILNP Comparison</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uqt8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>17uqoer</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Matte Polish Top Coat</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz2khxltt70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>17uq8a4</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Let my boyfriend pick the colors for my skittles mani, I think he did well :)</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec96lo3yp70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>17uq3s3</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Cotton candy 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uq3s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>17uq0fw</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Cats In The Cradle featuring Mochi (swipe for pics)!</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uq0fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>17uq082</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>A moment of silence before I trim my index down😔</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xvxq6g1o70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>17upxc6</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>mooncat - velvet rose🎀</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17upxc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>17up8f3</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Is this too much?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17up8f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>17uosd3</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Opinions on scented quick dry top coats?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17uosd3/opinions_on_scented_quick_dry_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>17uoqvy</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Moment of appreciation for Mooncat’s Enchanted Mist 😍</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uoqvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>17uocqw</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>For those of you shopping your collection - some great for Fall 2022 Cirque Colors multichromes.</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wkj21z5y970c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>17unv5t</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Extreme purple glow</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17unv5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>17unurr</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>MC Blame My Star Sign + Cirque Jellies = ❤️</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twh93ldz570c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>17unooe</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Winter-y Sweater Nails 🩵❄️</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17unooe</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>17unkrm</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Tips for applying leaf glitters like this? The edges keep raising for me</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw7717fy370c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>17un7js</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Difference between Cirque Colors Rose and Rosewater Jellies?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17un7js/difference_between_cirque_colors_rose_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>17un05v</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Got my Mooncats and test results!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17un05v</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>17umzjc</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Blue - Silver Mani with Sabertooth accent</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17umzjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>17umujs</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Finally got my Mooncat order!!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhitvb18y60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>17um2ms</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>stars handpainted by me!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zav43fxbs60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>17ulubk</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Enchanted polish — Forks, WA</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ulubk</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>17ulmw3</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Bowery by Cirque Colors - much darker and redder on me than I expected 🤔</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4csx3m6p60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>17uleu8</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Wasatch Yellow Iron Ore in the Wasatch Range UT</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kedktikn60c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>17ulb7p</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Scrappy FOMO fall mani</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ulb7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>17ukaj2</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Vibrant Autumn 🍃</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ukaj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>17ujz6l</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Testing Out My New Toppers</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ujz6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>17ujwm3</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Cadillacquer The Sea of Sands</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ujwm3/cadillacquer_the_sea_of_sands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>17uj3ts</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Twinkle nails.</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uj3ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>17uj106</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Fade Into You - Beaux Reeves</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srvnkcbt560c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>17ui48v</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Thermals can take everything I have</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xbzu8tqxy50c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>17ui3zr</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Blue Monday</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/IdrCPDB</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>17uhumn</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Monday sadness 😭</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsq8x87zw50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>17uh0kx</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Forever in love with the timeless charm of pink nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/getyfrohq50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>17ugtu6</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Setup</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rip8b8n2p50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>17ufzhz</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Weekly Check-In for those on a low buy/no buy, etc.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ufzhz/weekly_checkin_for_those_on_a_low_buyno_buy_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>17ufvk7</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Green day. Catrice - Believe in Jade</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8m8fhd9rh50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>17uf0py</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My attempt to duplicate mooncat on a no-buy!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uf0py</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>17ueh92</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>I‘m looking for a nail polish that looks like the nail foils on the screenshot (source: ebruerguener on IG)</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/moryo5is650c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>17ue7jq</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Milky White &amp; Pink</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ue7jq/milky_white_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>17udzl2</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Orly - Country Club Khaki + Color Club - Wake Up Call</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17udzl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>17udunb</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Bad Seed by DVN</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17udunb</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>17udepw</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>My first holo mani and I can’t stop looking at my nails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17udepw</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>17ucp1f</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Tinted base coat</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ucp1f/tinted_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>17ucbei</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>it’s getting chilly bundle up. 🥶❄️✨</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy0p0l7bp40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>17uc8un</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Esmaltes Da Kelly (EDK) polish in the UK?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17uc8un/esmaltes_da_kelly_edk_polish_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>17uc2g3</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>{PR} Love these combos 💕</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q855nxh3n40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>17u88zd</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17u88zd/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>17us4mq</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Fall nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17us4mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>17urbba</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I love my new naillll</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fi26nchz70c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>17upugo</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>What’s the difference between 3d, 5d and 9d cat eye gel polishes? In terms of how they look and/or what effects you can achieve with them?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17upugo/whats_the_difference_between_3d_5d_and_9d_cat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>17umwf6</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What’s on my hands this week as a nail tech</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17umwf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>17um6py</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Animal inspired Autumn</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17um6py</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>17uhy82</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Took on the clown nails challenge 💅 How’d I do? Did them on myself 🤡✨</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyb1ttxpx50c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>17uhm4p</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Wrecked my design..but whatever</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uhm4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>17uccqz</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>My nail girl Esthetics by Katie in Nova Scotia killin’ it once again 😍</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x9sqgllp40c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>17u6zyl</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Nightmare on Elm Street</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/30tgf425330c1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov 15 08:08:25 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C467"/>
+  <dimension ref="A1:C607"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8370,6 +8370,2386 @@
       <c r="C467" t="inlineStr">
         <is>
           <t>https://v.redd.it/30tgf425330c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>17vje3r</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Picked up this glitter top coat today and no matter how long I cure it's still tacky. Bottle doesnt day no wipe but also doesnt say it needs to be wiped. Anyone have experience with this brand? Did I do an oops and get one that needs alcohol wipe?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4a89b6raf0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>17voq69</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>I miss doing my nails, it’s been MONTHS! Decided on shorties this time around! 💅🏽</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w9vmagewg0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>17vom1w</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>went all out at the nail salon 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vom1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>17vgde7</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Help! Nails not lasting! Gel chipping on natural and false nails always lifting?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5i2uxcnske0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>17vey5r</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Tortoise and Croc inspired.</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbxxh51h9e0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>17venm1</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>green and silver nails! cat eye, chrome, and aura</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17venm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>17vdi44</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>First time trying French tips</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vdi44</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>17voe4j</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>First duck set</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17voe4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>17vod9k</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>best nail shape for beach volleyball?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vod9k/best_nail_shape_for_beach_volleyball/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>17vob5s</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>how do nail techs achieve this look?</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prjk0tdtqg0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>17vny5b</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>I never got e very good photo of these. Which is a shame bc I love them sm.🐄</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vny5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>17vnivc</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Just thought these ladies deserved a moment 🙌🏼</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol3nrci2hg0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>17vcqq8</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Why are my nails peeling towards the tips?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk1qq0jqsd0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>17vn2ea</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>been a while since i've had acrylic nails!! do these look ready for a fill?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vn2ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>17vmwad</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqgerout9g0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>17vmsy9</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Frequent fills?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vmsy9/frequent_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>17vmlem</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Finally got my nails done again after 3 months they aren't perfect but I love them ❤️</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6ggx3ec6g0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>17vlxsu</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Smart or Dumb</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vlxsu/smart_or_dumb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>17vlfsj</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>A couple of designs I tried out today!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a58azn1wtf0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>17vley5</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>I usually want a monochromatic manicure, but I decided to add variety and make this design. There are white seagulls on the big nail.</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jenskufysf0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>17vleln</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">self taught nail tech </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2a9wprsjtf0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>17vlaww</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>"Little Red Corvette" 🏎️ by me!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fm1nfcicsf0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>17vl1d2</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Polish coming off whole</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vl1d2/polish_coming_off_whole/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>17vk0ry</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>marble 💙</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vk0ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>17vjcw9</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Something fun for upcoming Turkey Day. 🦃💍👑</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b3e6ijd8af0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>17vj5ie</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>A manicure I got in China for less than $25 (USD)</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vj5ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>17vj0g3</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Natural nail length!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnu1qlpd7f0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>17viwsj</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Index nails are spoon shaped, and keep getting caught in things, please help</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17viwsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>17vioep</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Sistaco - do I need the set</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vioep/sistaco_do_i_need_the_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>17vinfu</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Why do these look so bad 😞?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vinfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>17vijzr</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Which shape and length is best?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vijzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>17vihh4</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Some birthday nails! Scorpio baby</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7141ais2f0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>17vi4bi</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>September &amp; October ☺️</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vi4bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>17vhij2</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>From mess to manicured. My autumn nails transformation today. 💅🤎🍂</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vhij2</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>17vhhta</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Beautiful early Christmas nails! I love that it’s so sparkly</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vhhta</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>17vg4e3</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Princess Zuko from Avatar The Last Airbender 🔥</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vg4e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>17vg1s7</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>all pink mani &amp; pedi!!! 🎀</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vg1s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>17vffdk</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>First time using TGB biab ✨</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmshbdd6de0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>17vf3bh</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Nail wraps on artificial nails?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vf3bh/nail_wraps_on_artificial_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>17velat</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Cuticle oil favs?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17velat/cuticle_oil_favs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>17vek5s</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>As a 31yo lifetime nail biter and picker, I was shocked at my natural length after my last gel set was drilled off!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nvlb3cg6e0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>17vclwf</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Getting dirty looks at the nail salon as a man</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vclwf/getting_dirty_looks_at_the_nail_salon_as_a_man/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>17vcbap</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Do you think long or short nails are better on my hands? Certified nail tech - I do them myself 😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2kr1zripd0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>17vb5c2</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Product suggestions for flat nails?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlwzl2jofd0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>17vbk46</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Dip Nails falling apart quickly</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vbk46/dip_nails_falling_apart_quickly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>17vb8kh</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Nails bending too easily, what can I do?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vb8kh/nails_bending_too_easily_what_can_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>17vap2e</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Second set of French in my life 💅</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vap2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>17va6sk</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>The longest my nails have ever been 🥹 I’m so proud</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17va6sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>17v9img</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Minimalist fall nails 🍁</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z17oadms2d0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>17v8ye5</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>I want to try a dark color on my nails, but I love these fun bright colors! Decisions, decisions.</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vp6uihhyc0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>17v7q76</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Tried some press on nails, but now I have questions. I’ve tried glue on nails, but can’t get them to last more than 24 hours. However, these press on are going on day five with minimal lifting.</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0lvr11ioc0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>17v7gld</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Need help with my natural nails!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v7gld</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>17v705t</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Mooncat polishes are so mesmerizing 💜</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v705t</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>17v6rfa</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Ferrari red🔥</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy0o1fkjhc0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>17v6nr8</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Hoping this reaches the right audience 🙏</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17v6nr8/hoping_this_reaches_the_right_audience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>17v6fi0</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Gift Suggestion for My Wife?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17v6fi0/gift_suggestion_for_my_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>17v6fhb</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>I'm a mooncat convert.</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v6fhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>17v3tue</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>polish chipping off</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e25kijptb0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>17v67wp</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>I wanted bling 💅🏻</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v67wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>17uuslr</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>how do i fix these damaged monstrosities?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uuslr</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>17uuoln</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>how do i make them more square? also could use general advice on nail &amp; cuticle care please!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uuoln</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>17v5r2i</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>DND Walnut Brown and some gold foil!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apiaftnh9c0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>17v5qr7</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>First time doing square, thoughts?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v5qr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>17v59vc</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g38yoemo5c0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>17v4k1d</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Rate my work!</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v4k1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>17v4f5i</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Tips for at home manicure tools</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17v4f5i/tips_for_at_home_manicure_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>17v4e3z</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>A little sparkle before Thanksgiving</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yrucsxcyb0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>17v3zht</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Silk 💜🤗</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98i56p71vb0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>17v3rzn</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>White gel for nail art recommendations?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6bg9zc8tb0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>17v3i71</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>sage green 🍃🌿🌱</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tf0eq3uqb0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>17v3h2o</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>im a snow fairy! 🥶🧚🏾‍♀️🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v3h2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>17v3ay1</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Slowly getting better at doing my own nails! Tips or feedback are appreciated!!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxdnlgn4pb0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>17v1tij</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>first time using chrome powder!!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v1tij</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>17v0pua</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Jade Stone 💚🩵🤍</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tutufkl5za0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>17v0h7r</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>A bit much? I think not 😆 ok maybe 👀</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ki853cvbwa0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>17v0del</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Why can't people take zoomed in pictures of their nails? Do we need to see 90% of the background?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17v0del/why_cant_people_take_zoomed_in_pictures_of_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>17uzahn</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>which color and shape suit me best? it’s for a wedding, will glue tabs stay on? (Picture 1 and 2 are the same)</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17uzahn</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>17uyl9x</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Fml….</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyzoi33s7a0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>17uyhu0</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Ive never had almond/stiletto nails, only coffin. Do you think almond nails would look better or do i stick with the coffin?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3myj093f6a0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>17vortw</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Mooncat foxfire</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd0imy21xg0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>17vn53u</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>seche vite bubbling and does not go on smooth. Can nail polish go bad?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekd8wselcg0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>17vltbc</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Which of these boutique &amp; indie brands last the longest for you?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vltbc/which_of_these_boutique_indie_brands_last_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>17vlmss</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Ironic💚💙</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vlmss</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>17vljor</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>What white glitter polish should I buy?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mll23ge3vf0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>17vl9db</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>What do you think of this color combination?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzthqsourf0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>17vkwfs</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>"Sapphire tears with the iced out wrist" by me!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vkwfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>17vkkwh</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Low-key Pumpkins with a Dash of Petals by me (ig: beowoofstudio)</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sttfyucljf0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>17vka44</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>2nd Haul from the Mooncat Sale 🙈😆💕</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vka44</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>17vjysy</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Ilnp Mayfield vs looking glass</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vjysy</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>17vjul2</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Grandma says you can do Halloween nails now.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vjul2</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>17vjimr</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>2 Months ago this sub was recommend to me. Now I’m making DIY nail oil pens.</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vjimr</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>17vjfo9</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Space-y magnetics ⭐️✨</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vjfo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>17vj06a</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Mooncat house of hades question</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vj06a/mooncat_house_of_hades_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>17viulf</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Before &amp; After Getting Even Nail Primer by Mooncat 🌜😻</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17viulf</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>17vicef</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>enjoying this ballerina pink moment 🩷</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vicef</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>17vhvqu</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Will OPI Nail Envy work if you remove it regularly?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vhvqu/will_opi_nail_envy_work_if_you_remove_it_regularly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>17vhkc3</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Mooncat Haul</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gz2xvyhque0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>17vh3p2</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Thank you all for your feedback on my last mani! This is a pre-cleanup shot (because I always manage to smudge during cleanup) of my 2nd attempt at rainbow nails. CCW! 🌈💅🏻</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uap8u4auqe0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>17vgs7n</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>My first ever attempts at nail art! 🍄🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vgs7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>17vg6v2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Who else LOVES cutting down to shorties?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9nxvnpdje0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>17vfzbq</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>[pr] holo taco - after party!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vfzbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>17vfqrq</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Looking for a liquid nail glue that isn't too strong</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vfqrq/looking_for_a_liquid_nail_glue_that_isnt_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>17vfhce</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Unexpectedly Love This Combo</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vfhce</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>17velbs</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Yikes in a professional cookbook, AITA?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vla3lwp6e0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>17vdhfu</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>My first of a bajillion winter nails ❄</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wh5qqy6yd0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>17vdc2i</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Follow up to my troubleshooting call from Jill with Glisten &amp; Glow: surprise gift!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/375aniz4xd0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>17vd879</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Matte shimmer... That GLOW ❤</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vd879</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>17vd4pb</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Quick “between sets” refresh</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vd4pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>17vbh6x</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Night sky nails</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1wgaqjyid0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>17vau7u</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Tortoiseshell</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vau7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>17vafi8</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>House of Hades swatches</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqrjx8v1ad0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>17v9zt2</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Velvetized Mooncat Velvet Rose💖</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zotza2ki6d0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>17v9jol</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>First time in a long while that I’ve painted my nails!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v9jol</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>17v8p2j</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Any Montreal Laqueristas want to team up for Holo Taco haul?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17v8p2j/any_montreal_laqueristas_want_to_team_up_for_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>17v85qx</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Mooncat Fall Skittle</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v85qx</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>17v7xjo</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Gold and Lavender stamps by me</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v7xjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>17v7o2y</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>All In 💚 Cirque Colors X KelliMarissa</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v7o2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>17v7f83</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Swamp Gloss Pretty on the Inside 🤩</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v7f83</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>17v6yw2</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>OPI It’s a Girl!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v6yw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>17v6sel</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Mooncat haul came in, Thanksgiving mani, and a quick cuticle question!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v6sel</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>17uyg0m</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>What are your thoughts on men who enjoy doing makeup or engaging in 'cute' activities like painting their nails for fun?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhdvry0q5a0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>17v5mif</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Where did I go wrong…</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1vyuibg8c0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>17v5amy</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Mooncat Pangea… it’s okay.</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9b41ghu5c0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>17v53x9</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Mostly unlabeled Color Club skittle nails</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vmmakqa4c0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>17v4shv</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>sunset magic ✨</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v4shv</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>17v4fzl</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Should I wash off acetone before polish?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17v4fzl/should_i_wash_off_acetone_before_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>17v3kb6</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>im a snow fairy! 🥶🧚🏾‍♀️🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v3kb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>17v3dkk</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Cobalt with toppers</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/rlrNWgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>17v3c47</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Holo sparkle in the sun &gt;&gt;&gt; anything else</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlrdrxoepb0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>17v0miy</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>ILNP is still the MVP</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/IRoVIWK</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>17uzqkm</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>A moment of appreciation while at work</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzg6lwv7na0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>17vksj3</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>"Rainbow's end, a feline friend" by me! (ig: @beowoofstudio)</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vksj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>17vg3uk</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Zuko from Avatar The Last Airbender 🔥🔥</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vg3uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>17vceca</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Leaving for vacation in 2 days. Should I repaint?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd1vqr74qd0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>17vb0sx</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Lil homie! @GBB_Nails</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oecwmygped0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>17vazes</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Lil Homie! @gbb_nails</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vazes</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>17vaou9</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Made these nails for a friend with a little black cat named "Booper".</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk7onoy3cd0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>17v9ao7</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I'm like a magpie with these...🐦‍⬛</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v9ao7</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>17v7vxx</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>I did these nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv970kebqc0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>17v48uo</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>First try with painting...</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17v48uo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov 16 08:08:29 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C607"/>
+  <dimension ref="A1:C750"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10750,6 +10750,2437 @@
       <c r="C607" t="inlineStr">
         <is>
           <t>https://www.reddit.com/gallery/17v48uo</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>17whgjc</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>any idea how to make nails grow thicker ?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17whgjc/any_idea_how_to_make_nails_grow_thicker/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>17wbggu</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Nail frustration- what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wbggu/nail_frustration_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>17wgqvn</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Love soft pinks🌸</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gusnueosn0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>17wfqez</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Aura Nails with Eyeshadow?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eispkqpphn0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>17wfbca</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>How often do you find yourself checking out your nails in a day?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wfbca/how_often_do_you_find_yourself_checking_out_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>17weykk</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>New🌼</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygm03v2k9n0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>17weplg</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Freestyle for my client!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17weplg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>17we48o</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Charged for shape?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17we48o/charged_for_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>17wdsql</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Trying aura nails!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpu30u7mym0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>17wdn8z</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>How are we feeling about these animal print nails that I did on myself?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iszpbjx6xm0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>17wc7gp</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9se085vkm0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>17wc51x</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Best beginner nail set yet</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wc51x</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>17wbpm6</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>My best beginner nails yet!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wbpm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>17wbm2u</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>2 weeks wear before and after!</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wbm2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>17wb52y</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Grooming day! Rounder shape test. Yay or nay? I usually go for a more square shape.</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nk4gzw6cm0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>17wanbw</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Polygel</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijb4kla88m0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>17w9w4u</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t xml:space="preserve">there is never enough brightness </t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dxqrcnmb2m0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>17w993r</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Nail Art Design (Cinderella)</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w993r</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>17w8nol</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>First time I get my nails done and I can't stop checking them out. Thoughts? 🤭</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9bsvkgiqsl0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>17w8jsi</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Did my fall nails today🧡🖤💛</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zngernxrl0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>17w88f0</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Fixing chipped nails</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17w88f0/fixing_chipped_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>17w7z1x</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>thanksgiving nails! 🌼</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w7z1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>17w7izh</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Today’s nails. It’s all free hand by Mia at Jenna’s</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnab8gv9kl0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>17w7bos</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>I'm loving this plaid!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69zbg4msil0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>17w703v</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Do I have long or short nail beds?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6y6u7cjgl0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>17w62ll</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>(Male) Cuticle too hard to remove</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17w62ll/male_cuticle_too_hard_to_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>17w5ydk</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Channeling a return to spooky season. Paparazzi Polish / Tango Star</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg875d449l0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>17w5r7f</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Decided to try some new colors and nail art</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w5r7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>17w46un</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Did my birthday nails today🎂</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fb7ol5qwk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>17w3y4i</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Found the nail tech of my dreams.🥺</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kk7zv0yuk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>17w3xmp</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>nails for the new Hunger Games movie!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w3xmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>17w3ux8</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>The last time I posted it was the longest set I had ever gotten, just got them done and these are even longer 😍</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w3ux8</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>17w3u8z</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Some Autumn Sloth Nails</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w2yz2k6uk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>17w38ho</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Reusable nails</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17w38ho/reusable_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>17w36pd</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Soft pink chrome on natural shorties - I got my dream nails while vacationing in Whistler.</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47bbw5m6pk0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>17w2zg1</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>From a while back, still one of my favourite</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16bobz7nnk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>17w29zt</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>How did I do on these homemade press-ons??? I want to eat them... 😳</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnxim7iaik0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>17w2fqw</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>💗In love with my nails 💕</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6to7gwgjk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>17w2esg</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>my cat themed nails 😸</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yosy17u9jk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>17w29dr</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Help! My nail polish never stays on for more than a day without chipping. Any idea why?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w29dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>17w2383</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Need Recommendations:Newbie At Gels Preparing For Black Friday Sales</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17w2383/need_recommendationsnewbie_at_gels_preparing_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>17w1lb5</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Recovering Nail Biter &amp; Cuticle Picker</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w1lb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>17w1hu2</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w1hu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>17w1gut</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>First time trying Gelx and I'm so happy with the results!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w1gut</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>17w1g8x</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>I'm OBSESSED with this polish from mooncat "MERKITTEN"</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1oqrqorbk0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>17w1cnj</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Barbie Opalescence 💕💕💕</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e08yznxyak0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>17w0owl</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Good apex?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjuxzkbt5k0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>17w01jc</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>The longest my natural nails have ever been! Went with something sheer to celebrate the length 💖</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t03khit0k0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>17vzygs</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Is there way to make it look smoother at home?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0alykk70k0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>17vzxmy</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Another week a new set of press ons 😌☃️❄️</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vzxmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>17vzr0s</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Full coverage help</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01lb6ftmyj0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>17vzbf2</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Please help me choose a nail dust collector</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vzbf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>17vxtyz</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Guys how do I make my nails look good again after years of biting</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vxtyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>17vvkld</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Flat/uneven hard gel ?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vvkld</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>17vydf5</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>We need a green butterfly emoji…</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vydf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>17vsfh4</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Want longer nails on my natural nails</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vsfh4/want_longer_nails_on_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>17vrq51</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Where to learn about acrylics?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vrq51/where_to_learn_about_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>17vl6uy</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Any apps that let you try nail colours and nail shapes on your hands?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17vl6uy/any_apps_that_let_you_try_nail_colours_and_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>17vuv64</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>First time using rhinestones!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vuv64</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>17vuoka</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Are gel top coats meant to be gummy?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ceageivnti0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>17vttk9</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Witchcult Lacquer - Welcome to Silent Hill</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vttk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>17vt93w</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Need advice!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyzlvf4bgi0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>17vt27w</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Trying to make my on press ons and they turned out weird?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n8t0f8gei0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>17vqy0v</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Sea on the nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vqy0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>17vq9k1</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Autumn 🍂/ thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vq9k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>17whe8y</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Finally tried out one of the “designer” techs and LOVE my nails</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17whe8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>17wh3o5</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Advice- My nails have been square shaped so long on some of my fingers that my skin has shaped to it, is there a fix?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wh3o5/advice_my_nails_have_been_square_shaped_so_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>17wg3od</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>it's been almost 2 and a half years since my nail started to grow wide like this, can it still be fixed?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zexv8k2kln0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>17wfk86</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Anyone else love swatching their collection?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt0wjo40gn0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>17wdbfj</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>I got too excited for the holidays and did Christmas nails too early</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wdbfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>17wcw84</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Nail Polish Abroad?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wcw84/nail_polish_abroad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>17wc9bc</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Favorite Glow Polishes</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wc9bc/favorite_glow_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>17wbzom</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Cirque Colors- Au</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wbzom/cirque_colors_au/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>17wbp3k</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Mooncat weeping willow</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hyv6t0mgm0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>17wbozq</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Favorite Nail Polish of ALL TIME?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2d35wtlgm0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>17wbj2i</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Essie creme</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soj387iafm0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>17wb5m3</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Rate My Mani</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wb5m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>17watbg</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Can I see your fave periwinkle/cornflower blue polish?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17watbg/can_i_see_your_fave_periwinklecornflower_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>17wa78x</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Macchiato Cloud ☕️☁️</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wa78x</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>17w91zm</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Painted my short nails with holo</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bryko0sqvl0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>17w8c90</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>It’s… beautiful</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3drs34hbql0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>17w77gm</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Eric, Wherever You Dwell</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w77gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>17w72fv</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Mooncat- Mercury’s Tears</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w72fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>17w6kzi</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Early chipping/tip wear - base coat or top coat issue?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17w6kzi/early_chippingtip_wear_base_coat_or_top_coat_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>17w673h</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Baby’s first magnetics</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yj7eo5fxal0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>17w5z7i</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Frostbite</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w5z7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>17w5o3p</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Cirque Colors Introverde + Pixie Holo ✨🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w5o3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>17w5h2r</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Very happy with first mooncat order</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brs1ctfx5l0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>17w5d01</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>A collab with the sideboard forest 🌲✨️</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w5d01</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>17w43wx</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Neutral nails for a gloomy day ☁️</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w43wx</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>17w42qd</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Mooncat Poseidon’s Prize while I wait for my sale order</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w42qd</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>17w3r0b</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Some Autumn Sloth Nails</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpcxw7hitk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>17w3589</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>The perfect natural pink</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17w3589/the_perfect_natural_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>17w10gi</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>What are some of your all-time favorite jellies or sheers?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17w10gi/what_are_some_of_your_alltime_favorite_jellies_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>17w2ke0</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Making the most of fall colors before the holidays</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds4b1ksfkk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>17w1wvv</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Double Fall</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w1wvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>17w1vfu</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Back in business with my sparkly self! 💖</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bngz3364fk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>17w1co8</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>autumn skittles</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w1co8</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>17w0yfw</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>What's a good (your favourite) way to store polishes that might be available in Canada and doesn't cost an arm and a leg? 🤣😁</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17w0yfw/whats_a_good_your_favourite_way_to_store_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>17w0tms</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Mooncat formula rant</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17w0tms/mooncat_formula_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>17w0kka</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>DVN Nocturnal dupe?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17w0kka/dvn_nocturnal_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>17w0d1x</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>House of hades mooncat</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w0d1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>17w06n9</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Always had short, soft brittle nails. After 2 months of TLC I'm super happy at where they are today 😊</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/202x1exv1k0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>17w05yc</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Shroomdom</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w05yc</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>17vzung</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>the closest i can get to a fall look with my current collection (feat. my deeply lazy right hand!)</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vzung</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>17vzr18</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Zoya Haul Report!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vzr18/zoya_haul_report/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>17vz041</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>SYS - Weekly Challenge #1 - Ooh, what is this? ✨👀</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70fb0xozsj0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>17vy7z7</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Probably my first "fancy schmancy" mani I've done</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byxye3cxmj0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>17vy1in</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>time for another monthly mani roundup + honest reviews!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vy1in</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>17vxy8i</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Ethereal- Maui</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/yEk689D</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>17vxlmv</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>The Quintet ✨</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vxlmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>17vxe4c</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Polish a big streak-y?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vxe4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>17vmvy2</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>made a gradient with pearlescent pigment powder :D</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vmvy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>17vx3s9</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Navy, cobalt, indigo swatch comparison Cirque</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vx3s9/navy_cobalt_indigo_swatch_comparison_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>17vwzmg</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>{PR} In love 💕</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufrool91dj0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>17vwt5p</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Sèche Vive?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vwt5p/sèche_vive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>17vwshu</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Has Mooncat ever recreated LLP’s Kraken?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jj83ixdbj0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>17vvo1g</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Update: Where did I go wrong</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbrro3v62j0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>17vvbgr</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Mooncat spaceoddity</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vvbgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>17vv2u6</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>nail growth and cuticles since finding this sub🥹🙏🏻💓</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vv2u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>17vunq7</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Painted last night, used QDTC and getting dents today??</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qwoz30cti0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>17vumo1</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Orly - Olive You Kelly + SH Xtreme Wear - Strobe Light</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vumo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>17vu719</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>How do you guys clean your brushes?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17vu719/how_do_you_guys_clean_your_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>17vtrre</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Witchcult Lacquer - Welcome to Silent Hill</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vtrre</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>17vtrgc</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Does anyone know of any polishes similar to this? Very new to painting my nails and I’m in love with how this one reflects the light :)</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/divhnfhbli0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>17vtr8s</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Love the shiftiness</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihrbxzb9li0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>17vtj1s</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>wanted to share my first proper attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9h34qy1ji0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>17vq5xr</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>My nail polish collection 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vq5xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>17vppyy</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>At the park and my nails are GLOWING</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zgek0np9h0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>17vpm9m</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>I couldn’t decide which polish to wear from this collection so I wore them all</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vpm9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>17whbhe</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>cartoon heart design I got a little while ago at ChiChi Nails in Ontario 💕💕</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dom5smogzn0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>17wha8k</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Christmas is coming fast ❄️☃️ 🎄 😭 here’s a hand drawn snowflake design done at ChiChi Nails in Ontario . 💅</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0spbdcp1zn0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>17wh4mi</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>What are your nail art tips for a beginner?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17wh4mi/what_are_your_nail_art_tips_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>17weywo</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>hello kitty press on set by me (ig: nailsbylilari)</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvyvfiuz9n0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>17w5m84</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Plaid and sweater nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9z7qd29x6l0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>17w3sky</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Some Autumn Sloth Nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5186xk4utk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>17w2ykx</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Trying a new design</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyx89c0hnk0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>17w1mhd</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Simple Fall nails by meee</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17w1mhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>17w1f8x</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Jellies! I used a Tortoise Shell kit from KoKoist for the torties.</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol2jmwrjbk0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>17vzr2q</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>First Christmas nails of the season</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tg514xboyj0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>17vyava</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>best iPhone camera for close up nail videos? iPhone X &gt; IPhone 13 Pro Max?!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/moy71bcgnj0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>17vvvyq</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Indoors vs. outdoors ✨</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vvvyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>17vrasv</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>My best Halloween nails so far!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17vrasv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov 17 08:08:17 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C750"/>
+  <dimension ref="A1:C892"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13181,6 +13181,2420 @@
       <c r="C750" t="inlineStr">
         <is>
           <t>https://www.reddit.com/gallery/17vrasv</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>17xa91a</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>I broke a nail really bad it to the inside but now I’m using it as an example nail</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhnu4mze8v0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>17x9hzx</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Press-on/gel-x help</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x9hzx/pressongelx_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>17x8em2</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Holiday nails with the red bottoms</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x8em2</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>17x8drg</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Fresh Fall Nails</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x8drg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>17x88y7</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>How to get glue off press ons?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x88y7/how_to_get_glue_off_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>17x84yr</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Do you have to use a magnet with cateye polish</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x84yr/do_you_have_to_use_a_magnet_with_cateye_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>17x83vr</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Back at it with the fresh neon nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72dri181iu0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>17x7nre</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I wish these wouldn’t grow out 😩</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x7nre</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>17x771x</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Got a manicure while in Seoul!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj1ro9a68u0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>17x770z</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Set I made for one of my students 😊</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0byu0268u0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>17x6nz5</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Any tips on how to get closer to the edge/should I?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cd8yi7n2u0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>17x6dbr</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>New nails 💅</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x6dbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>17x64fy</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>You can tell my nail tech was rushing, but I don’t mind! I was the last customer of the day. Plus she refused to take a tip.</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyke8yg1xt0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>17x62om</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>I Think I'm Keeping the Almond Shape!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94spym7hwt0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>17x5x67</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x5x67/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>17x5aht</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Painted my nails pink</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8k19fv4ipt0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>17x4pvc</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>tried water marbling for the first time</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cbp3igjkt0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>17x4g1v</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Nails I did a couple of weeks ago... got fill em but was requested to share ❤️</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy3b54w7it0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>17x3i01</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>What is this technique and why do I only see this done in asia?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gi5vvcy9t0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>17x2p8y</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>how we like these</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kavvzga83t0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>17x2g23</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>How do we feel about this shape on me?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x2g23</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>17x2d0a</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>One of my first pro manicures</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x2d0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>17x14vk</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Fresh set, loving it….. what do you think?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llnlt4uhqs0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>17x0t70</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>I tried to do gradient nails and failed lmao</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x0t70</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>17x0o52</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x0o52/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>17x0e8l</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Is this full set worth 110$? Chop shop too I love them but never paid this much there before so just curious what others think</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x229t6uqks0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>17wzsk6</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Pink and gold sparkle with charms</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n52kldd6gs0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>17wzl9n</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>My newest set after 3 weeks of growth</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wzl9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>17wz86h</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>winter blues ❄️ the argyle nail is my favorite :)</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00a2eueybs0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>17wz3ib</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Cosy season means sweater nails. Did them myself and love how they turned out.</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqfhwms0bs0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>17wz2yq</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Jelly nails</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg3shzfwas0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>17wyut6</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>memories of my dark past lol</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z8al1w79s0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>17wyim5</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Maroon moment</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5e98pbo6s0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>17wy04w</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Just painted my (early) birthday nails!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wy04w</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>17wxepq</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Renaissance vibes</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54sdhltdyr0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>17ww8qz</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>At home nail kit recommendations please</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ww8qz/at_home_nail_kit_recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>17ww14r</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Quick Rant :(</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ww14r</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>17wvzxk</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Chrome, glitter and french mani all in one 🩷</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gkmwqqbnr0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>17wvvzo</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Ignore my shaking I have lupus and anxiety 😆 I wanted to show y’all them on! 🥰 press on set by me 🥰</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/njl645bimr0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>17wvwhw</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>First time trying chrome</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wvwhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>17wvqq9</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>My first mooncat order! Had to start with Sand Viper 🌙🐈✨</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wvqq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>17wvmmn</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>I love how they turned out!!! Most are gel but the glitter is acrylic. Luxury press Ons are where it’s at!!!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wvmmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>17wvfyq</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>I might be having too much fun with this set, do you like the collab?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32zpz7z0jr0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>17wuucc</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>I went neutral for this manicure. I love them</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wuucc</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>17wulwm</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>First time I do my nails(alone at home). Can you correct the mistakes and give me more tips ( best shape for my hands etc ..)</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lo5vb9hcr0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>17wucyv</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🎂</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qylw1sakar0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>17wu21l</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>New nail day!!</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qokpehb68r0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>17wt7ed</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>cow print french tips 🐮🤠</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fs5t41k1r0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>17wt527</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Favorite Brands For Rubber Base, Gels and Magnetic Polish?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0v7we011r0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>17wszmn</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>I'm in love with this new set! 💅🏻</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wszmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>17wsw72</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>What’s the silliest way you’ve broken a nail?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wu2jpqzyq0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>17wsqgm</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>All of my nails are breaking!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wsqgm/all_of_my_nails_are_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>17wse6z</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Best glue on nails?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wse6z/best_glue_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>17wr2l9</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Frustrates</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wr2l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>17ws0f6</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Send your need to get nail supplies!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17ws0f6/send_your_need_to_get_nail_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>17wk4at</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Pastel flower nail art 🌸</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wk4at</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>17wrx9r</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Trying to master the “velvet” effect 🌚 🔮 (excuse my shaky hands)</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fc8j4skerq0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>17wqr28</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Shorties can be really cute and practical</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdw2pchsiq0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>17wq09w</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>it's starting to get hard to take out my contacts so I think I found the limit on my natural nails</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8annjbbidq0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>17wpv5e</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Sorry in advance if this is a dumb question…</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wpv5e/sorry_in_advance_if_this_is_a_dumb_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>17wol2m</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I love the design, do you like it?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i64ga2iq2q0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>17wnpa8</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Rate my nail tech!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5g18naqvp0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>17wnoy1</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>DIY Fall Set</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wnoy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>17wne9a</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>New set, little bit bobbly in places as its cold in my house so taking a long time to dry. Maybe time to invest in a lamp perhaps?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7gfdhgctp0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>17wnabe</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Heart of the gold</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvww246hsp0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>17wn5ae</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>In my shorty era</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wn5ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>17wn3s0</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Help with nails flipping</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wn3s0/help_with_nails_flipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>17wmf13</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>My nails are making people question their sanity</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wmf13</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>17wlyyk</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Trying new colours! What do you think?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3avqwwhwgp0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>17wlot2</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Product suggestion for thin cracked nails ( of an octogenarian)</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wlot2/product_suggestion_for_thin_cracked_nails_of_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>17wli05</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Birthday nail ideas?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wli05</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>17wkj9x</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Nothing too special. Just sharing what mine look like this week 💅</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8pjhvfb2p0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>17wkdam</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>second time doing gel on myself 🩷</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wkdam</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>17wjyx4</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Just pure nude goodness</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wjyx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>17wjikp</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Red nails</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p61e65stqo0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>17wiw5z</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>How to do lettering on nails? Polish and techniques?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17wiw5z/how_to_do_lettering_on_nails_polish_and_techniques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>17x9l77</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Has anyone tried this brand?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4np7gdpuzu0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>17x80af</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Obsessed with this subtle purple</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/miod4fixgu0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>17x7vzw</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Yet another House of Hades post</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eki1t3nfu0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>17x7a2v</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Newbie to the nail world</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17x7a2v/newbie_to_the_nail_world/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>17x77jr</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Are Cirque Hygge and Morningtide different enough for me to get both?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17x77jr/are_cirque_hygge_and_morningtide_different_enough/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>17x71k5</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Any tips on how to get closer to the edge/should I?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmpaah4k6u0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>17x5rsu</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Mooncat Lunar Eclipse Order finally came in 🤭</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x5rsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>17x5ex7</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Baby-Approved Glitter 👶✨️🌟</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwnptjnhqt0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>17x574y</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Waterless manicure</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17x574y/waterless_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>17x3s1a</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>First holo taco order!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iylt3bpcct0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>17x3io1</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>I heard we were sharing House of Hades nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x3io1</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>17x2vg6</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Any idea what color this is?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x2vg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>17x2ptd</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>I’m very satisfied with how my first lil gems are holding up</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x2ptd</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>17x1ivq</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>October &amp; November nails</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x1ivq</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>17x1eyw</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Any swatches of A Comet's Tail by Sassy Sauce?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggers8fsss0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>17x0ghe</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I’ve been out of work for less than a week. so obviously i change my nails everyday.</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x0ghe</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>17wzz5x</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>House of Hades</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2b6ydvkhs0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>17wzuee</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>In love with my first mooncat mani</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6wux5cyjgs0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>17wz80x</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Zoya Bisoux, part of the Magical (holiday 2023) collection</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wz80x</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>17wyr40</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Tis the season, what is your favorite winter holiday polish?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wyr40/tis_the_season_what_is_your_favorite_winter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>17wy4iv</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Least favorite nail products?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brw22esp3s0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>17wxxuw</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Heartless wench vs. dark horse feat. color coordinating weiner dog</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wxxuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>17wxhuz</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>First time trying at home gels turned out pretty well!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1ktp6m1zr0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>17wxahe</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Need a dupe for mooncats Kiss My Asteroid....</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wxahe/need_a_dupe_for_mooncats_kiss_my_asteroid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>17wwp4p</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>I saw a comet 💫</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wwp4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>17wwi55</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>This one threw me off guard - in a good way LOL</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lr21dlarr0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>17wwhdn</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>HOW TO GROW NAIL BACK</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wwhdn/how_to_grow_nail_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>17wvsi2</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My first mooncat order! Had to start with Sand Viper 🌙🐈✨</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wvsi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>17wvngd</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Y'all are bad influences 😂</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnckpyjokr0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>17wvnay</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Mooncat - Moonjelly at the gas station</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pqzswunkr0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>17wv2jz</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Natural pink</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wv2jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>17wusz5</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Help Finding a Polish</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wusz5/help_finding_a_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>17wu6vz</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Chanel La Base Camelia Issue</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wu6vz/chanel_la_base_camelia_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>17wtvh2</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Crackling Fire</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qwsno6qp6r0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>17wtowm</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>new polish for my bday!!🌈</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wtowm</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>17wtgha</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>{PR} The GLOW 😍</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zih3r4jh3r0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>17wt190</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Latest manicures with new square-ish shape. Which shape do you prefer? CCW</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wt190</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>17wsv09</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Gentleman Pirate and Fools Gold</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uqf3enqyq0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>17wsiyc</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Can’t have long nails anymore so I’m trying tips!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2njmb45wq0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>17wrn0c</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>For those who voted matte topper</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wrn0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>17wrmh2</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Any tips on preventing my nails from splitting into layers? Or at least on preventing myself from peeling them off...</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wrmh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>17wr18t</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>mooncat shipping</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wr18t/mooncat_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>17wqtw3</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Glass frog</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wqtw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>17wqq31</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>What pink do you think would work with Mooncat's Smokescreen?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wqq31/what_pink_do_you_think_would_work_with_mooncats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>17wqlf4</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>ILNP Poppy</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wqlf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>17wq3jg</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Mooncat is replacing my defective Pangea ✨</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dpwakd6eq0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>17wq0m8</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Fall flowers done bad, lol. I On Nails, Orly BB Cream Barely Blanc, Expressie Seize The Minute(red), Sinful Colors Hot Toffee(brown), Essie Meet Me At Sunset(orange), Orly Snow White and finished with Essie Speed-Setter.</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wq0m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>17wp1nc</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Work casualty...</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wp1nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>17wo88m</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Sharing my happiness!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9vhawxwzp0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>17wms03</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Cirque Dream within a dream</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wms03</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>17wlxvi</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Classic 🖤🤍🖤</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wlxvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>17wlht7</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Please send help- My nails and hands are completely wrecked, I need some advice on a care routine for my nails and possibly hands!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wlht7</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>17wkzbx</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Ilnp/cirque comparison</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17wkzbx/ilnpcirque_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>17wkthg</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Experimenting with a new (to me) colour combination for autumn</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wkthg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>17wkgqi</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Matte or glossy? Difficult to decide 🙈</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wkgqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>17x96k2</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Advice/product recommendations to get this raised chrome look (inspo by @suzu_nails on ig)</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x96k2</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>17x76qx</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Made a set for one of my students 13th birthdays 🥳</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p13at138u0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>17x4fhs</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I cried after my last nail appointment</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x4fhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>17x3rb1</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>favorite art of the day</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owuiram6ct0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>17wzg0u</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Pumpkin Fall</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wzg0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>17wvrdr</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Press on set done by me (TikTok-Bratitude Nails) 💕</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9cfhip2ilr0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>17wvomu</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>I love how they turned out!!! Luxury press ons are where it’s at!!!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wvomu</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>17wpo57</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Gel nails I did on a friend 🐱</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wpo57</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>17wpgkm</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Birthday nails for me, by me</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wpgkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>17wkouu</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Tried dome swirly nails 💜✨</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wkouu</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>17wk3c2</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Pastel flowery set 🌸</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17wk3c2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov 18 08:07:26 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_19.xlsx
+++ b/data/2023_11_19.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C892"/>
+  <dimension ref="A1:C1046"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15595,6 +15595,2624 @@
       <c r="C892" t="inlineStr">
         <is>
           <t>https://www.reddit.com/gallery/17wk3c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>17y1gjc</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I want my nails redone</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oevr2o21a21c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>17y16lv</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>I made myself these Gel Press Ons 🤩🤎🍷🧡</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6florjlg621c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>17y0s1u</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>In my own pink world</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17y0s1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>17y0q76</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>My second attempt at rubber gel nails.</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17y0q76</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>17y0i5t</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Suggestions?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17y0i5t/suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>17y0d30</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Forest butterfly nails!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17y0d30</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>17xzy6x</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>My girls getting bored with one color</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xzy6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>17xyjat</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Whatcha think?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5luti8izb11c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>17xy7ru</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Do you like my nails? 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7klauil811c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>17xy2eo</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>In love with it! 🩷</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5721sro0711c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>17xy1z5</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>How to keep press on nails from popping off?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r89w1evv611c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>17xxikt</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Builder Gel Nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa0nqyxc111c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>17xwd5h</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Trying to be more creative with my nails, is this cute? I like it but idk</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xwd5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>17xwcdz</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Best builder gel / build in a bottle gel?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xwcdz/best_builder_gel_build_in_a_bottle_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>17xw5t2</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Work in progress 😁🧼</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0x29qti4p01c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>17xw258</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Best press ons for wide nail beds?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xw258/best_press_ons_for_wide_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>17xvtew</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cgmcts1m01c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>17xvb47</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>White streak on my nail with tiny black specks. Could it be leukonychia?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qb7wpr6h01c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>17xu4yc</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Did I get scammed..?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c781ld6i701c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>17xtzjk</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Neutral matte nails.</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xtzjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>17xtwwd</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Chopped them after the wedding</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xtwwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>17xtsbi</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>☯️</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufig0wjj401c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>17xtgj0</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Red 24/7</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xtgj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>17xsvb3</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>I loved my new nails.</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/0LQjyQ0.gifv</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>17xsotu</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Tried Dip for the first time</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xsotu</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>17xs739</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>It’s giving vampire Christmas 🧛‍♀️🎄 newest set done by me</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nkcpb4jmrz0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>17xr0ts</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>SpongeBob Nailsss 🧽</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxyublshiz0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>17xr00y</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Nail Dip Removal</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xr00y/nail_dip_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>17xqv58</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Good quality nail art brush</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xqv58/good_quality_nail_art_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>17xqgif</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Fresh set!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yii3fy47ez0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>17xqfkc</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Never back down never what</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xqfkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>17xqfb4</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Dark Winx Club set I did for Halloween 🖤🖤🖤</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xqfb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>17xpew1</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Soak off &amp; Mani</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xpew1/soak_off_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>17xq40d</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Do most salons not do corkscrew nails? (@kiaraskynails)</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xq40d/do_most_salons_not_do_corkscrew_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>17xpwvo</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>My nail artist is truly a gem. Been seeing her for nearly 3 years and she never disappoints!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xpwvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>17xpu5t</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Which shape suits me? 1 or 2?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xpu5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>17xox1t</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>| which is best? |</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4ldnxzc2z0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>17xou5u</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Thoughts on my nails.</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssllr6iq1z0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>17xopn4</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>I bought some nail glue, but its completely dried up, is there anything I can do?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xopn4/i_bought_some_nail_glue_but_its_completely_dried/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>17xoods</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Nude pink with gold accents</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xoods</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>17xnb1y</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Pure acetone?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xnb1y/pure_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>17xn52b</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Classic 🖤🤍🖤</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xn52b</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>17xmzi6</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Does my nail shape look strange?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xmzi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>17xmqh1</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Nail stamping advice</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xmqh1/nail_stamping_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>17xm96j</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Holy grail products/brands, please!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xm96j/holy_grail_productsbrands_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>17xm6bj</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I am a hungry hungry …</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w76yxmp9gy0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>17xm1p2</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>First ever attempt at doing my nails. Any advice?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xm1p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>17xlok3</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>I think they are my fav now</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xlok3</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>17xj3c2</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Ready for the holidays! Gingerbread cookie inspired nails 🤎</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvpw2psrrx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>17xllac</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>first attempt at glitter ombre</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xllac</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>17xlcjq</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>What shape suits my hands better?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xlcjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>17xl42d</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Who said press-ons were for kids again?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xl42d</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>17xky54</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Why is this happening?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg0w0t6k6y0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>17xkqdx</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Woodland nails ft. the cutest lil' mushrooms (by charlylouisebeauty)</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujrudfmt4y0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>17xk4p5</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Recent manicure</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wghihqxzx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>17xjr3h</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Introverted/ Socially Anxious nail techs, how do deal with the small talk with your clients, especially new one.</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xjr3h/introverted_socially_anxious_nail_techs_how_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>17xj9b8</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails! My artist always makes my visions come true! </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eim67vwzsx0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>17xj9le</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Glow in the dark beauties</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xj9le</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>17xchxi</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>My Cruella De Vil inspired nails</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzjmhqvn2w0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>17xj1qx</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu5e1vgerx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>17xj1ah</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Does anyone have any recommendations for drugstore red nail polishes that go well with really pale skin with blue/ purple undertones?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xj1ah/does_anyone_have_any_recommendations_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>17x5dca</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>first post here; assorted, semi-freestyle nails! ❤️🤎 first time doing french tips too!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x5dca</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>17x5bjq</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Another fill!!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x5bjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>17x4jy6</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Beginners drill?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x4jy6/beginners_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>17xiy13</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Fall nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mozvxufjqx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>17xig1y</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>tortie</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/255gsgohmx0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>17xidge</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Reflective polish is so 😍</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xidge</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>17xibwc</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>What am I doing wrong with my nail polish?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plvepngklx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>17xibf0</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>😮‍💨 Can't have them too long without breaking</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sot23huglx0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>17xi8eh</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Tragedy 😞</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xi8eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>17xi7vw</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Nails Newbie</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xi7vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>17xh68f</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>How are my acrylics?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/atrs3ff3cx0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>17xh4p9</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Finally was able to do a fall set! I don’t hate it 😆 the lines are tricky but fun!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i87cuddqbx0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>17xgvmc</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I cried a bit... Nobody at work could understand</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xgvmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>17xguhn</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Browns for Thanksgiving 🤎</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kyf4ohg9x0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>17xgqc8</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>The press-ons I’ll keep for the weekend</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xgqc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>17xgbnn</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>My new set I did, I like them!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h53s977w4x0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>17xedwu</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>do you like my manicure?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pb905ybnw0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>17xdj5f</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>The most creative set i have ever had</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xdj5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>17xd8d9</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Getting rid of my favourite set ever this weekend 😭</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyk0rnzyaw0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>17xczk9</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Has anyone tried Jello Jello tip off gel?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17xczk9/has_anyone_tried_jello_jello_tip_off_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>17xco96</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Shape question…</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xco96</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>17x25es</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Dip powder or gel overlay?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75e5dr9pys0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>17x0llf</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>A magical, low maintenance manicure routine (please)</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17x0llf/a_magical_low_maintenance_manicure_routine_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>17x0h77</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>poor nails :( how do I fix them?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17x0h77</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>17y0ron</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>I don't understand jelly sandwiches, help!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17y0ron</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>17y0r20</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>In my own pink world</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17y0r20</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>17y01ba</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Black ice set</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17y01ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>17xuc9m</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>First time using polygel fill in</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xuc9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>17xy7lr</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Swatch request - Deep Space and Mad Hatter</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xy7lr/swatch_request_deep_space_and_mad_hatter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>17xy36x</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Subdulous - LynB</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xy36x</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>17xy24d</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>LynB order arrived!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xy24d</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>17xxz7m</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Pour one out for me</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71t573f2611c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>17xxurz</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Lucky Jelly: six day streak and going strong</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xxurz</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>17xxou7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Not my usual colour, but thought I’d give it a go 🩵💙</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7wb9t95311c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>17xx9ru</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>My first try at magnetic nail polish!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhwngdo2z01c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>17xx2pd</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Gotta love jellies 🤩✨</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ge9au3e9x01c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>17xw0bw</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Matched my favorite cup.</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6gjmzyrn01c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>17xtqh2</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Blue or Purple?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xtqh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>17xsboi</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>More Blue</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xsboi</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>17xrt8t</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>After months of Holo nails I decided to go in the opposite direction</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv77j9zioz0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>17xqny3</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Creams vs. Sparkles (Zoya 10 for $25)</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xqny3</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>17xqfpb</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>my latest “mani”</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59pqxh80ez0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>17xq6pk</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Is there a Zoya dupe for mooncat's "Pangea"?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xq6pk/is_there_a_zoya_dupe_for_mooncats_pangea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>17xq6en</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>What is this cloth in Essie Nail Tool Duo used for?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0x11k2a2cz0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>17xpqs5</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Orly Black Friday</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xpqs5/orly_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>17xoxjx</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Water Decal Success thanks to u/GargantuanGreenGoats</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xoxjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>17xox8q</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Fave LE release of all time?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xox8q/fave_le_release_of_all_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>17xoog2</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Zoya 10 for $25 haul</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihd6mgef0z0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>17xo5tw</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>They look infrared!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cvttc95wy0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>17xo4mu</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Loud Lacquer brush replacements?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd35pirvvy0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>17xnqz4</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>I'm just a girl in the world...</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xnqz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>17xmyz1</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Late to the party, but brought my personal Latte Cloud along</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqr77y7kmy0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>17xmtbq</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Prugly green recommendation</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xmtbq/prugly_green_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>17xmqcg</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Hiding the short nails with literal perfection over here</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sh6eyvppky0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>17xmm3d</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>It Finally Feels Like Fall in Texas</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2sd3dyrjy0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>17xlzd4</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Cadillacquer with gel top</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xlzd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>17xlyne</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Came back from a trip but left behind a piece of my nail at the airport</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmz7tqyley0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>17xlwsb</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>A couple glittery looks I’ve had lately ✨</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xlwsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>17xlt4h</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Mooncat: your heart is a black hole</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xlt4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>17xlplq</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Thoughts on Lacquer22</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xlplq/thoughts_on_lacquer22/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>17xlc59</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Finally got my order!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okuuek3m9y0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>17xktrx</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for Polished for Days The Wanderer</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7r32axk5y0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>17xkmxx</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>What is up with ILNP</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xkmxx/what_is_up_with_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>17xkkrw</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Pretty… but I’m also pretty sure I hate them? 😂</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xkkrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>17xkj17</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Wide brush compatible with Witchcult?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xkj17/wide_brush_compatible_with_witchcult/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>17xkg9e</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Is there a way to emphasize the non-magnetic parts of a magnetic polish?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xkg9e/is_there_a_way_to_emphasize_the_nonmagnetic_parts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>17xk3mw</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Wasn’t ready for all this jelly!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xk3mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>17xjwci</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Has anyone’s Zoya order actually shipped yet?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xjwci/has_anyones_zoya_order_actually_shipped_yet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>17xjm53</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>My first thermal! “Northern Light My Fire” by LynB Designs</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ylhe8sxvx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>17xjk6k</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>What I have with me for 5 Months of Travel and Very Little Space!</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xjk6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>17xjju4</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>A hoodwink feat air bubbles 🙄</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/PvXNBSa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>17xinhq</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Second time doing a full set of polygels. Only took a quick 4+ hours 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwurwlc5ox0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>17xiinl</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Artemis’ Deathkiss ⚰️ 💋</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xiinl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>17xhwqr</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>(Sassy Sauce Polish) Cock_a_doodle_Doom</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nizpi4xhx0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>17xhshg</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Poser 💚</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xhshg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>17xhs4h</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Should I switch salons?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xhs4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>17xhifu</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Fishnet Stockings</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/depmxowtex0c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>17xhbj0</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Pumpkin pie nails</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw15ar7bdx0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>17xh5dh</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>hard to capture just how shifty this one is ✨💧</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xh5dh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>17xg0yt</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Twisted Terracotta Tanzanite is wild</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xg0yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>17xfott</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Mooncat Dark Horse</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xfott</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>17xe4t6</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Here for the Boos</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l30372iokw0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>17xci47</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>YAY</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exstdgjq2w0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>17xbfgf</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>How to use swatch sticks best</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17xbfgf/how_to_use_swatch_sticks_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>17xb1e2</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Clean girl ✨</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xb1e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>17xztul</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Avocado Nails</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xztul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>17xvgee</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Gold Nail</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gob99e6xi01c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>17xqwp2</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Newest mani 🧡</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17xqwp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>17xquny</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Good quality nail art brushes</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17xquny/good_quality_nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>17xqj21</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dfrm0ppez0c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>17xknvk</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Woodland nails ft. the cutest lil' mushrooms (by charlylouisebeauty)</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhaui8d94y0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>17xifu1</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Red Jelly</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/999bf5qfmx0c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>17xfsig</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love motion in my nails. Just put this set in a hurry, I'm self taught. CCW </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1wdbyiph0x0c1</t>
         </is>
       </c>
     </row>

</xml_diff>